<commit_message>
Separation des cours d'anglais
</commit_message>
<xml_diff>
--- a/Q1/Modelisation_evenement/Prises_de_notes/Exdercice_1.xlsx
+++ b/Q1/Modelisation_evenement/Prises_de_notes/Exdercice_1.xlsx
@@ -8,14 +8,51 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clementpotier/Downloads/test/IG2-C/Q1/Modelisation_evenement/Prises_de_notes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{49235DED-0323-3B4C-B91C-C1FDA3951482}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{691CAE0E-2EA8-A041-827C-9CC42E2DFC9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{1276EF01-715A-9644-B926-205D25A72D84}"/>
+    <workbookView xWindow="300" yWindow="500" windowWidth="27000" windowHeight="16940" xr2:uid="{1276EF01-715A-9644-B926-205D25A72D84}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <definedNames>
+    <definedName name="solver_adj" localSheetId="0" hidden="1">Feuil1!$C$2:$C$3</definedName>
+    <definedName name="solver_cvg" localSheetId="0" hidden="1">0.0001</definedName>
+    <definedName name="solver_drv" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_eng" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_itr" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_lhs1" localSheetId="0" hidden="1">Feuil1!$C$7</definedName>
+    <definedName name="solver_lhs2" localSheetId="0" hidden="1">Feuil1!$C$8</definedName>
+    <definedName name="solver_lhs3" localSheetId="0" hidden="1">Feuil1!$C$9</definedName>
+    <definedName name="solver_lin" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_mip" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_mni" localSheetId="0" hidden="1">30</definedName>
+    <definedName name="solver_mrt" localSheetId="0" hidden="1">0.075</definedName>
+    <definedName name="solver_msl" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_neg" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_nod" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_num" localSheetId="0" hidden="1">3</definedName>
+    <definedName name="solver_opt" localSheetId="0" hidden="1">Feuil1!$C$12</definedName>
+    <definedName name="solver_pre" localSheetId="0" hidden="1">0.000001</definedName>
+    <definedName name="solver_rbv" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rel1" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rel2" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rel3" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rhs1" localSheetId="0" hidden="1">Feuil1!$D$7</definedName>
+    <definedName name="solver_rhs2" localSheetId="0" hidden="1">Feuil1!$D$8</definedName>
+    <definedName name="solver_rhs3" localSheetId="0" hidden="1">Feuil1!$D$9</definedName>
+    <definedName name="solver_rlx" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rsd" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="solver_scl" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_sho" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_ssz" localSheetId="0" hidden="1">100</definedName>
+    <definedName name="solver_tim" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_tol" localSheetId="0" hidden="1">0.01</definedName>
+    <definedName name="solver_typ" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_val" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="solver_ver" localSheetId="0" hidden="1">2</definedName>
+  </definedNames>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -531,7 +568,7 @@
   <dimension ref="A1:XFD1048575"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="O20" sqref="O20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -546,7 +583,7 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>2.9999999999999996</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -554,7 +591,7 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -568,7 +605,7 @@
       </c>
       <c r="C7">
         <f>C2+3*C3</f>
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="D7">
         <v>18</v>
@@ -580,7 +617,7 @@
       </c>
       <c r="C8">
         <f>C2+C3</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="D8">
         <v>8</v>
@@ -592,7 +629,7 @@
       </c>
       <c r="C9">
         <f>2*C2+C3</f>
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="D9">
         <v>14</v>
@@ -609,37 +646,37 @@
       </c>
       <c r="C12">
         <f>C2+1.5*C3</f>
-        <v>0</v>
+        <v>10.5</v>
       </c>
     </row>
     <row r="1048550" spans="16384:16384" x14ac:dyDescent="0.2">
-      <c r="XFD1048550" t="e" cm="1">
+      <c r="XFD1048550" cm="1">
         <f t="array" ref="XFD1048550">solver_pre</f>
-        <v>#NAME?</v>
+        <v>9.9999999999999995E-7</v>
       </c>
     </row>
     <row r="1048551" spans="16384:16384" x14ac:dyDescent="0.2">
-      <c r="XFD1048551" t="e" cm="1">
+      <c r="XFD1048551" cm="1">
         <f t="array" ref="XFD1048551">solver_scl</f>
-        <v>#NAME?</v>
+        <v>2</v>
       </c>
     </row>
     <row r="1048552" spans="16384:16384" x14ac:dyDescent="0.2">
-      <c r="XFD1048552" t="e" cm="1">
+      <c r="XFD1048552" cm="1">
         <f t="array" ref="XFD1048552">solver_rlx</f>
-        <v>#NAME?</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1048553" spans="16384:16384" x14ac:dyDescent="0.2">
-      <c r="XFD1048553" t="e" cm="1">
+      <c r="XFD1048553" cm="1">
         <f t="array" ref="XFD1048553">solver_tol</f>
-        <v>#NAME?</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="1048554" spans="16384:16384" x14ac:dyDescent="0.2">
-      <c r="XFD1048554" t="e" cm="1">
+      <c r="XFD1048554" cm="1">
         <f t="array" ref="XFD1048554">solver_cvg</f>
-        <v>#NAME?</v>
+        <v>1E-4</v>
       </c>
     </row>
     <row r="1048555" spans="16384:16384" x14ac:dyDescent="0.2">
@@ -649,39 +686,39 @@
       </c>
     </row>
     <row r="1048556" spans="16384:16384" x14ac:dyDescent="0.2">
-      <c r="XFD1048556" t="e" cm="1">
+      <c r="XFD1048556" cm="1">
         <f t="array" ref="XFD1048556">solver_ssz</f>
-        <v>#NAME?</v>
+        <v>100</v>
       </c>
     </row>
     <row r="1048557" spans="16384:16384" x14ac:dyDescent="0.2">
-      <c r="XFD1048557" t="e" cm="1">
+      <c r="XFD1048557" cm="1">
         <f t="array" ref="XFD1048557">solver_rsd</f>
-        <v>#NAME?</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1048558" spans="16384:16384" x14ac:dyDescent="0.2">
-      <c r="XFD1048558" t="e" cm="1">
+      <c r="XFD1048558" cm="1">
         <f t="array" ref="XFD1048558">solver_mrt</f>
-        <v>#NAME?</v>
+        <v>7.4999999999999997E-2</v>
       </c>
     </row>
     <row r="1048559" spans="16384:16384" x14ac:dyDescent="0.2">
-      <c r="XFD1048559" t="e" cm="1">
+      <c r="XFD1048559" cm="1">
         <f t="array" ref="XFD1048559">solver_mni</f>
-        <v>#NAME?</v>
+        <v>30</v>
       </c>
     </row>
     <row r="1048560" spans="16384:16384" x14ac:dyDescent="0.2">
-      <c r="XFD1048560" t="e" cm="1">
+      <c r="XFD1048560" cm="1">
         <f t="array" ref="XFD1048560">solver_rbv</f>
-        <v>#NAME?</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1048561" spans="16384:16384" x14ac:dyDescent="0.2">
-      <c r="XFD1048561" t="e" cm="1">
+      <c r="XFD1048561" cm="1">
         <f t="array" ref="XFD1048561">solver_neg</f>
-        <v>#NAME?</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1048562" spans="16384:16384" x14ac:dyDescent="0.2">

</xml_diff>